<commit_message>
Code is now complete
</commit_message>
<xml_diff>
--- a/Day13/Final.xlsx
+++ b/Day13/Final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="80">
   <si>
     <t>BANNU, PAKISTAN</t>
   </si>
@@ -22,12 +22,21 @@
     <t>PKBNP</t>
   </si>
   <si>
+    <t>BANNU PAKISTAN</t>
+  </si>
+  <si>
+    <t>ADD : BANNU PAK</t>
+  </si>
+  <si>
     <t>BUNER, PAKISTAN PASSPORT NUMBER: BA5496713</t>
   </si>
   <si>
     <t>PKBUN</t>
   </si>
   <si>
+    <t>BUNER PAKISTAN</t>
+  </si>
+  <si>
     <t>ADD : DERA GHAZI KHAN PAK</t>
   </si>
   <si>
@@ -40,6 +49,9 @@
     <t>PKGRT</t>
   </si>
   <si>
+    <t>GUJRAT, PAKISTAN PASSPORT NO.AE1805423</t>
+  </si>
+  <si>
     <t>ADD: GUJRANWALA, PAK PP# VE1164982</t>
   </si>
   <si>
@@ -64,12 +76,36 @@
     <t>PKKHI</t>
   </si>
   <si>
+    <t>KARACHI PAKISTAN CNIC NO 42201 3304868 7</t>
+  </si>
+  <si>
+    <t>PAKISTAN KARACHI USED CAR DEALER</t>
+  </si>
+  <si>
+    <t>KARACHI PAKISTAN</t>
+  </si>
+  <si>
+    <t>ADD : KARACHI PAKISTAN.</t>
+  </si>
+  <si>
+    <t>KARACHI PAKISTAN CNIC # 51401-9294445-3</t>
+  </si>
+  <si>
+    <t>KARACHI PAKISTAN CNIC # 43205-1404594-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFICE NO.601,ISMAIL TRADE CENTRE, JODIA BAZAR,KARACHI </t>
+  </si>
+  <si>
     <t>LAHORE,PAKISTAN.</t>
   </si>
   <si>
     <t>PKLHE</t>
   </si>
   <si>
+    <t>ADDRESS: HOUSE NO. : 410 BLOCK A MOUALLAH GULSHAN RAVI, LAHORE PAKISTAN.</t>
+  </si>
+  <si>
     <t>ADD:FAISALABAD,PAKISTAN CNIC # 33102-2420365-3</t>
   </si>
   <si>
@@ -85,7 +121,25 @@
     <t>MARDAN PAKISTAN</t>
   </si>
   <si>
-    <t>DIR UPPER PAKISTAN</t>
+    <t xml:space="preserve">DIR UPPER PAKISTAN </t>
+  </si>
+  <si>
+    <t>DIR PAKISTAN</t>
+  </si>
+  <si>
+    <t>ADD DIR UPPER PAK</t>
+  </si>
+  <si>
+    <t>DIR LOWER, PAKISTAN</t>
+  </si>
+  <si>
+    <t>DIR LOWER, PAK</t>
+  </si>
+  <si>
+    <t>ADD : LOWER DIR PAK PASSPORT # JJ1170991</t>
+  </si>
+  <si>
+    <t>ADD : DIR LOWER PAK PASSPORT # AM0724942</t>
   </si>
   <si>
     <t>MULTAN,PAKISTAN</t>
@@ -115,18 +169,33 @@
     <t>PKPEW</t>
   </si>
   <si>
+    <t>ADD: PESHAWAR, PAK PP NO: PC4123151</t>
+  </si>
+  <si>
     <t>RAWALPINDI, PAKISTAN</t>
   </si>
   <si>
     <t>PKRWP</t>
   </si>
   <si>
+    <t>RAWALPINDI ,PAK</t>
+  </si>
+  <si>
+    <t>RAWALPINDI PAKISTAN</t>
+  </si>
+  <si>
+    <t>RAWALPINDI,PAKISTAN</t>
+  </si>
+  <si>
     <t>RAHIM YAR KHAN, PAKISTAN</t>
   </si>
   <si>
     <t>PKRYK</t>
   </si>
   <si>
+    <t>RAHIM YAR KHAN PAKISTAN</t>
+  </si>
+  <si>
     <t>GOJRA TEH .MALIKWAL .DISTRICT MANDI BAHAUDDIN,PAKISTAN NIC : 34401-4367568-1</t>
   </si>
   <si>
@@ -139,16 +208,52 @@
     <t>PKSKT</t>
   </si>
   <si>
-    <t>ADD: SWABI PAKISTAN</t>
+    <t>SIALKOT, PAKISTAN PASSPORT NO. BL1609833</t>
+  </si>
+  <si>
+    <t>SIALKOT, PAKISTAN PASSPORT NO : ZR1791793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIALKOT, PAKISTAN </t>
+  </si>
+  <si>
+    <t>SIALKOT PAKISTAN</t>
+  </si>
+  <si>
+    <t>SIALKOT, PAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD: SWABI PAKISTAN </t>
   </si>
   <si>
     <t>PKSWB</t>
   </si>
   <si>
+    <t>ADD.SWABI PAK</t>
+  </si>
+  <si>
+    <t>SWABI PAKISTAN</t>
+  </si>
+  <si>
+    <t>ADD # SWABI PAKISTAN</t>
+  </si>
+  <si>
     <t>SWAT PAKISTAN</t>
   </si>
   <si>
     <t>PKSWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD: SWAT PAKISTAN </t>
+  </si>
+  <si>
+    <t>SWAT,PAKISTAN</t>
+  </si>
+  <si>
+    <t>ADD.SWAT PAK</t>
+  </si>
+  <si>
+    <t>ADDRESS# SWAT PAKISTAN PP# BC0722662</t>
   </si>
 </sst>
 </file>
@@ -480,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -499,87 +604,87 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -587,111 +692,615 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>44</v>
+      </c>
+      <c r="B60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>71</v>
+      </c>
+      <c r="B81" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>72</v>
+      </c>
+      <c r="B82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>74</v>
+      </c>
+      <c r="B84" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>74</v>
+      </c>
+      <c r="B85" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>